<commit_message>
Finished My Single Function
</commit_message>
<xml_diff>
--- a/CH-112 Custom Rank.xlsx
+++ b/CH-112 Custom Rank.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3278BB11-D69B-4838-AA31-FFECE3A229A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA7460-7E9E-41FF-B432-D77B71DC4CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt" sheetId="3" r:id="rId3"/>
+    <sheet name="MySingleFunction" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="10">
   <si>
     <t>Result</t>
   </si>
@@ -88,6 +89,9 @@
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7240101880893186048/</t>
   </si>
+  <si>
+    <t>Single Function</t>
+  </si>
 </sst>
 </file>
 
@@ -96,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:m"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +135,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -146,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -333,11 +344,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -395,8 +416,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1419,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66316581-FD42-47EA-B035-1A80E1D5A783}">
   <dimension ref="B1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1613,4 +1636,303 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D09A85D-B614-45CC-B4A9-5112DA9974E9}">
+  <dimension ref="C1:O23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.8984375" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.69921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.09765625" customWidth="1"/>
+    <col min="9" max="9" width="8.69921875" customWidth="1"/>
+    <col min="11" max="11" width="6.09765625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="K1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="21"/>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="3:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="15">
+        <v>2023</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10">
+        <v>35</v>
+      </c>
+      <c r="E3" s="11">
+        <v>99</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10">
+        <v>19</v>
+      </c>
+      <c r="E4" s="11">
+        <v>92</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="K4" s="12">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10">
+        <v>80</v>
+      </c>
+      <c r="E5" s="11">
+        <v>64</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="K5" s="12">
+        <v>3</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="10">
+        <v>92</v>
+      </c>
+      <c r="E6" s="11">
+        <v>80</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="K6" s="12">
+        <v>4</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="22" t="str" cm="1">
+        <f t="array" ref="C11:E15">C2:E6</f>
+        <v>Product</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H11" s="16" t="str" cm="1">
+        <f t="array" ref="H11:I11">K2:L2</f>
+        <v>Rank</v>
+      </c>
+      <c r="I11" s="16" t="str">
+        <v>Product</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="str">
+        <v>A</v>
+      </c>
+      <c r="D12" s="1">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1">
+        <v>99</v>
+      </c>
+      <c r="F12">
+        <f>E12-D12</f>
+        <v>64</v>
+      </c>
+      <c r="H12" s="12" cm="1">
+        <f t="array" ref="H12:H15">_xlfn.SEQUENCE(ROWS(C12:C15))</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="8" t="str" cm="1">
+        <f t="array" ref="I12:I15">_xlfn.SORTBY(C12:C15,F12:F15,-1)</f>
+        <v>B</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="str">
+        <v>B</v>
+      </c>
+      <c r="D13" s="1">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1">
+        <v>92</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F15" si="0">E13-D13</f>
+        <v>73</v>
+      </c>
+      <c r="H13" s="12">
+        <v>2</v>
+      </c>
+      <c r="I13" s="8" t="str">
+        <v>A</v>
+      </c>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="str">
+        <v>C</v>
+      </c>
+      <c r="D14" s="1">
+        <v>80</v>
+      </c>
+      <c r="E14" s="1">
+        <v>64</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="H14" s="12">
+        <v>3</v>
+      </c>
+      <c r="I14" s="8" t="str">
+        <v>D</v>
+      </c>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="str">
+        <v>D</v>
+      </c>
+      <c r="D15" s="1">
+        <v>92</v>
+      </c>
+      <c r="E15" s="1">
+        <v>80</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="H15" s="12">
+        <v>4</v>
+      </c>
+      <c r="I15" s="8" t="str">
+        <v>C</v>
+      </c>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="8:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="8:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="16" t="str" cm="1">
+        <f t="array" ref="H19:I23">_xlfn.VSTACK(K2:L2,_xlfn.HSTACK(_xlfn.SEQUENCE(ROWS(C3:C6)),_xlfn.SORTBY(C3:C6,E3:E6-D3:D6,-1)))</f>
+        <v>Rank</v>
+      </c>
+      <c r="I19" s="16" t="str">
+        <v>Product</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="12">
+        <v>2</v>
+      </c>
+      <c r="I21" s="8" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="12">
+        <v>3</v>
+      </c>
+      <c r="I22" s="8" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H23" s="12">
+        <v>4</v>
+      </c>
+      <c r="I23" s="8" t="str">
+        <v>C</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>